<commit_message>
Finished adding tests to results spreadsheet.
</commit_message>
<xml_diff>
--- a/DemoResults.xlsx
+++ b/DemoResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Test Name</t>
   </si>
@@ -22,9 +22,6 @@
     <t>Run time, ms</t>
   </si>
   <si>
-    <t>Copy records from Order</t>
-  </si>
-  <si>
     <t>Cursor</t>
   </si>
   <si>
@@ -37,27 +34,15 @@
     <t>Set-based</t>
   </si>
   <si>
-    <t>Subqueries</t>
-  </si>
-  <si>
     <t>Test #</t>
   </si>
   <si>
-    <t>In SELECT</t>
-  </si>
-  <si>
     <t>Rewrite as APPLY</t>
   </si>
   <si>
     <t>Rewrite as RowNum</t>
   </si>
   <si>
-    <t>In WHERE</t>
-  </si>
-  <si>
-    <t>User-Defined Functions</t>
-  </si>
-  <si>
     <t>Scalar UDF Data Access</t>
   </si>
   <si>
@@ -79,13 +64,52 @@
     <t>RowNum</t>
   </si>
   <si>
-    <t>Running Total</t>
-  </si>
-  <si>
     <t>Triangle Join</t>
   </si>
   <si>
     <t>Windowing</t>
+  </si>
+  <si>
+    <t>Sample run time, ms</t>
+  </si>
+  <si>
+    <t>Subquery</t>
+  </si>
+  <si>
+    <t>Subquery in SELECT (301,811 rows)</t>
+  </si>
+  <si>
+    <t>Subquery in WHERE (5,608 rows)</t>
+  </si>
+  <si>
+    <t>User-Defined Functions (13,147 rows)</t>
+  </si>
+  <si>
+    <t>~ ∞</t>
+  </si>
+  <si>
+    <t>Running Total (135,125 rows)</t>
+  </si>
+  <si>
+    <t>SSIS Price Update (7,515 rows)</t>
+  </si>
+  <si>
+    <t>Command Component</t>
+  </si>
+  <si>
+    <t>Staging</t>
+  </si>
+  <si>
+    <t>.NET App File Info Insert (10,000 rows)</t>
+  </si>
+  <si>
+    <t>Singleton Insert</t>
+  </si>
+  <si>
+    <t>SqlBulkCopy</t>
+  </si>
+  <si>
+    <t>Loops (301,811 rows)</t>
   </si>
 </sst>
 </file>
@@ -124,12 +148,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -144,11 +174,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,231 +489,379 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="3" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B3" s="2">
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>24421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B4" s="2">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>17668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B5" s="2">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>15058</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B6" s="2">
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B8" s="2">
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+      <c r="E8" s="3">
+        <v>4098</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B9" s="2">
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B10" s="2">
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B12" s="2">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="3">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B13" s="2">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B14" s="2">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B16" s="2">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3">
+        <v>217068</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B17" s="2">
+        <v>31</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B18" s="2">
+        <v>32</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="3">
+        <v>217076</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B19" s="2">
+        <v>33</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="3">
+        <v>217316</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B20" s="2">
+        <v>34</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B21" s="2">
+        <v>35</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B11" s="2">
+      <c r="E21" s="3">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B22" s="2">
+        <v>36</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B24" s="2">
+        <v>40</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3">
+        <v>8313</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B25" s="2">
+        <v>41</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B12" s="2">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B13" s="2">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B26" s="2">
+        <v>42</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="3">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B15" s="2">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B28" s="2">
+        <v>50</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="3">
+        <v>30279</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B29" s="2">
+        <v>51</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B31" s="2">
+        <v>60</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="3">
+        <v>87348</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B32" s="2">
+        <v>61</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B16" s="2">
-        <v>31</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B17" s="2">
-        <v>32</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B18" s="2">
-        <v>33</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B19" s="2">
-        <v>34</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B20" s="2">
-        <v>35</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B21" s="2">
-        <v>36</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B23" s="2">
-        <v>40</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B24" s="2">
-        <v>41</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B25" s="2">
-        <v>42</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>23</v>
+      <c r="E32" s="3">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A22:D22"/>
+  <mergeCells count="7">
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A23:E23"/>
   </mergeCells>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="84" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added demos for pre-materialization into temp tables.
</commit_message>
<xml_diff>
--- a/DemoResults.xlsx
+++ b/DemoResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Test Name</t>
   </si>
@@ -85,9 +85,6 @@
     <t>User-Defined Functions (13,147 rows)</t>
   </si>
   <si>
-    <t>~ ∞</t>
-  </si>
-  <si>
     <t>Running Total (135,125 rows)</t>
   </si>
   <si>
@@ -110,6 +107,12 @@
   </si>
   <si>
     <t>Loops (301,811 rows)</t>
+  </si>
+  <si>
+    <t>~ 31 hrs</t>
+  </si>
+  <si>
+    <t>Rewrite using #temp</t>
   </si>
 </sst>
 </file>
@@ -492,7 +495,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -521,7 +524,7 @@
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -612,41 +615,41 @@
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="3">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B11" s="2">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E11" s="3">
         <v>677</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B12" s="2">
-        <v>23</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="3">
-        <v>3171</v>
-      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B13" s="2">
         <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E13" s="3">
-        <v>3188</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
@@ -654,214 +657,236 @@
         <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="3">
-        <v>151</v>
+        <v>3188</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="B15" s="2">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1474</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B16" s="2">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="3">
-        <v>217068</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B17" s="2">
-        <v>31</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="3">
-        <v>161</v>
-      </c>
+      <c r="A17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B18" s="2">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E18" s="3">
-        <v>217076</v>
+        <v>217068</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B19" s="2">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E19" s="3">
-        <v>217316</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B20" s="2">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E20" s="3">
-        <v>2193</v>
+        <v>217076</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B21" s="2">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E21" s="3">
-        <v>2200</v>
+        <v>217316</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B22" s="2">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" s="3">
-        <v>156</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A23" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="B23" s="2">
+        <v>35</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="3">
+        <v>2200</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B24" s="2">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E24" s="3">
-        <v>8313</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B25" s="2">
-        <v>41</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B26" s="2">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E26" s="3">
-        <v>653</v>
+        <v>8313</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="B27" s="2">
+        <v>41</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B28" s="2">
+        <v>42</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="3">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B30" s="2">
         <v>50</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="3">
+      <c r="C30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="3">
         <v>30279</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B29" s="2">
-        <v>51</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="3">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A30" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B31" s="2">
+        <v>51</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B33" s="2">
         <v>60</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="3">
+        <v>87348</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B34" s="2">
+        <v>61</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="3">
-        <v>87348</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B32" s="2">
-        <v>61</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="3">
+      <c r="E34" s="3">
         <v>251</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A32:E32"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A25:E25"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="84" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="79" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add demo results spreadsheet from Baton Rouge.
</commit_message>
<xml_diff>
--- a/DemoResults.xlsx
+++ b/DemoResults.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -281,6 +281,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -316,6 +333,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -497,7 +531,9 @@
   </sheetPr>
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
@@ -538,7 +574,9 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3">
+        <v>15809</v>
+      </c>
       <c r="E3" s="3">
         <v>24421</v>
       </c>
@@ -550,7 +588,9 @@
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <v>10186</v>
+      </c>
       <c r="E4" s="3">
         <v>17668</v>
       </c>
@@ -562,7 +602,9 @@
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <v>9163</v>
+      </c>
       <c r="E5" s="3">
         <v>15058</v>
       </c>
@@ -574,7 +616,9 @@
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <v>161</v>
+      </c>
       <c r="E6" s="3">
         <v>172</v>
       </c>
@@ -595,6 +639,9 @@
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D8" s="3">
+        <v>3621</v>
+      </c>
       <c r="E8" s="3">
         <v>4098</v>
       </c>
@@ -606,6 +653,9 @@
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D9" s="3">
+        <v>3144</v>
+      </c>
       <c r="E9" s="3">
         <v>3395</v>
       </c>
@@ -617,6 +667,9 @@
       <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="D10" s="3">
+        <v>994</v>
+      </c>
       <c r="E10" s="3">
         <v>821</v>
       </c>
@@ -627,6 +680,9 @@
       </c>
       <c r="C11" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>500</v>
       </c>
       <c r="E11" s="3">
         <v>677</v>
@@ -648,6 +704,9 @@
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D13" s="3">
+        <v>2903</v>
+      </c>
       <c r="E13" s="3">
         <v>3171</v>
       </c>
@@ -659,6 +718,9 @@
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D14" s="3">
+        <v>2932</v>
+      </c>
       <c r="E14" s="3">
         <v>3188</v>
       </c>
@@ -670,6 +732,9 @@
       <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="D15" s="3">
+        <v>1547</v>
+      </c>
       <c r="E15" s="3">
         <v>1474</v>
       </c>
@@ -680,6 +745,9 @@
       </c>
       <c r="C16" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D16" s="3">
+        <v>224</v>
       </c>
       <c r="E16" s="3">
         <v>151</v>
@@ -701,6 +769,9 @@
       <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D18" s="3">
+        <v>183561</v>
+      </c>
       <c r="E18" s="3">
         <v>217068</v>
       </c>
@@ -712,6 +783,9 @@
       <c r="C19" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D19" s="3">
+        <v>104</v>
+      </c>
       <c r="E19" s="3">
         <v>161</v>
       </c>
@@ -723,6 +797,9 @@
       <c r="C20" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D20" s="3">
+        <v>194591</v>
+      </c>
       <c r="E20" s="3">
         <v>217076</v>
       </c>
@@ -734,6 +811,9 @@
       <c r="C21" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D21" s="3">
+        <v>184538</v>
+      </c>
       <c r="E21" s="3">
         <v>217316</v>
       </c>
@@ -745,6 +825,9 @@
       <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D22" s="3">
+        <v>1752</v>
+      </c>
       <c r="E22" s="3">
         <v>2193</v>
       </c>
@@ -756,6 +839,9 @@
       <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D23" s="3">
+        <v>1729</v>
+      </c>
       <c r="E23" s="3">
         <v>2200</v>
       </c>
@@ -766,6 +852,9 @@
       </c>
       <c r="C24" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="D24" s="3">
+        <v>265</v>
       </c>
       <c r="E24" s="3">
         <v>156</v>
@@ -787,6 +876,9 @@
       <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D26" s="3">
+        <v>4980</v>
+      </c>
       <c r="E26" s="3">
         <v>8313</v>
       </c>
@@ -798,6 +890,9 @@
       <c r="C27" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="D27" s="3">
+        <v>100000000</v>
+      </c>
       <c r="E27" s="3" t="s">
         <v>31</v>
       </c>
@@ -808,6 +903,9 @@
       </c>
       <c r="C28" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="D28" s="3">
+        <v>536</v>
       </c>
       <c r="E28" s="3">
         <v>653</v>
@@ -829,6 +927,9 @@
       <c r="C30" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="D30" s="3">
+        <v>3830</v>
+      </c>
       <c r="E30" s="3">
         <v>30279</v>
       </c>
@@ -839,6 +940,9 @@
       </c>
       <c r="C31" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="D31" s="3">
+        <v>271</v>
       </c>
       <c r="E31" s="3">
         <v>223</v>
@@ -860,6 +964,9 @@
       <c r="C33" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="D33" s="3">
+        <v>5061</v>
+      </c>
       <c r="E33" s="3">
         <v>87348</v>
       </c>
@@ -870,6 +977,9 @@
       </c>
       <c r="C34" s="2" t="s">
         <v>29</v>
+      </c>
+      <c r="D34" s="3">
+        <v>122</v>
       </c>
       <c r="E34" s="3">
         <v>251</v>

</xml_diff>

<commit_message>
Add results for Sioux Falls 2017.
</commit_message>
<xml_diff>
--- a/DemoResults.xlsx
+++ b/DemoResults.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -531,7 +531,7 @@
   </sheetPr>
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -575,7 +575,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="3">
-        <v>15809</v>
+        <v>13962</v>
       </c>
       <c r="E3" s="3">
         <v>24421</v>
@@ -589,7 +589,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="3">
-        <v>10186</v>
+        <v>10035</v>
       </c>
       <c r="E4" s="3">
         <v>17668</v>
@@ -603,7 +603,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="3">
-        <v>9163</v>
+        <v>8545</v>
       </c>
       <c r="E5" s="3">
         <v>15058</v>
@@ -617,7 +617,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="3">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="E6" s="3">
         <v>172</v>
@@ -640,7 +640,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="3">
-        <v>3621</v>
+        <v>3974</v>
       </c>
       <c r="E8" s="3">
         <v>4098</v>
@@ -654,7 +654,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="3">
-        <v>3144</v>
+        <v>3049</v>
       </c>
       <c r="E9" s="3">
         <v>3395</v>
@@ -668,7 +668,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="3">
-        <v>994</v>
+        <v>837</v>
       </c>
       <c r="E10" s="3">
         <v>821</v>
@@ -682,7 +682,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="3">
-        <v>500</v>
+        <v>446</v>
       </c>
       <c r="E11" s="3">
         <v>677</v>
@@ -705,7 +705,7 @@
         <v>19</v>
       </c>
       <c r="D13" s="3">
-        <v>2903</v>
+        <v>2881</v>
       </c>
       <c r="E13" s="3">
         <v>3171</v>
@@ -719,7 +719,7 @@
         <v>7</v>
       </c>
       <c r="D14" s="3">
-        <v>2932</v>
+        <v>2862</v>
       </c>
       <c r="E14" s="3">
         <v>3188</v>
@@ -733,7 +733,7 @@
         <v>32</v>
       </c>
       <c r="D15" s="3">
-        <v>1547</v>
+        <v>1294</v>
       </c>
       <c r="E15" s="3">
         <v>1474</v>
@@ -747,7 +747,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="3">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E16" s="3">
         <v>151</v>
@@ -784,7 +784,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="3">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="E19" s="3">
         <v>161</v>
@@ -826,7 +826,7 @@
         <v>14</v>
       </c>
       <c r="D22" s="3">
-        <v>1752</v>
+        <v>1833</v>
       </c>
       <c r="E22" s="3">
         <v>2193</v>
@@ -840,7 +840,7 @@
         <v>11</v>
       </c>
       <c r="D23" s="3">
-        <v>1729</v>
+        <v>1968</v>
       </c>
       <c r="E23" s="3">
         <v>2200</v>
@@ -854,7 +854,7 @@
         <v>15</v>
       </c>
       <c r="D24" s="3">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="E24" s="3">
         <v>156</v>
@@ -877,7 +877,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="3">
-        <v>4980</v>
+        <v>4743</v>
       </c>
       <c r="E26" s="3">
         <v>8313</v>
@@ -905,7 +905,7 @@
         <v>17</v>
       </c>
       <c r="D28" s="3">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="E28" s="3">
         <v>653</v>
@@ -928,7 +928,7 @@
         <v>25</v>
       </c>
       <c r="D30" s="3">
-        <v>3830</v>
+        <v>3642</v>
       </c>
       <c r="E30" s="3">
         <v>30279</v>
@@ -942,7 +942,7 @@
         <v>26</v>
       </c>
       <c r="D31" s="3">
-        <v>271</v>
+        <v>382</v>
       </c>
       <c r="E31" s="3">
         <v>223</v>
@@ -965,7 +965,7 @@
         <v>28</v>
       </c>
       <c r="D33" s="3">
-        <v>5061</v>
+        <v>851</v>
       </c>
       <c r="E33" s="3">
         <v>87348</v>
@@ -979,7 +979,7 @@
         <v>29</v>
       </c>
       <c r="D34" s="3">
-        <v>122</v>
+        <v>67</v>
       </c>
       <c r="E34" s="3">
         <v>251</v>

</xml_diff>

<commit_message>
Reset slide deck and spreadsheet for Kansas City 2017.
</commit_message>
<xml_diff>
--- a/DemoResults.xlsx
+++ b/DemoResults.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -281,23 +281,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -333,23 +316,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -531,8 +497,8 @@
   </sheetPr>
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -574,9 +540,7 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3">
-        <v>14055</v>
-      </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="3">
         <v>24421</v>
       </c>
@@ -588,9 +552,7 @@
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3">
-        <v>9446</v>
-      </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="3">
         <v>17668</v>
       </c>
@@ -602,9 +564,7 @@
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3">
-        <v>8743</v>
-      </c>
+      <c r="D5" s="3"/>
       <c r="E5" s="3">
         <v>15058</v>
       </c>
@@ -616,9 +576,7 @@
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3">
-        <v>157</v>
-      </c>
+      <c r="D6" s="3"/>
       <c r="E6" s="3">
         <v>172</v>
       </c>
@@ -639,9 +597,6 @@
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="3">
-        <v>2985</v>
-      </c>
       <c r="E8" s="3">
         <v>4098</v>
       </c>
@@ -653,9 +608,6 @@
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="3">
-        <v>3066</v>
-      </c>
       <c r="E9" s="3">
         <v>3395</v>
       </c>
@@ -667,9 +619,6 @@
       <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="3">
-        <v>853</v>
-      </c>
       <c r="E10" s="3">
         <v>821</v>
       </c>
@@ -680,9 +629,6 @@
       </c>
       <c r="C11" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D11" s="3">
-        <v>474</v>
       </c>
       <c r="E11" s="3">
         <v>677</v>
@@ -704,9 +650,6 @@
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="3">
-        <v>2812</v>
-      </c>
       <c r="E13" s="3">
         <v>3171</v>
       </c>
@@ -718,9 +661,6 @@
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="3">
-        <v>2832</v>
-      </c>
       <c r="E14" s="3">
         <v>3188</v>
       </c>
@@ -732,9 +672,6 @@
       <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="3">
-        <v>1311</v>
-      </c>
       <c r="E15" s="3">
         <v>1474</v>
       </c>
@@ -745,9 +682,6 @@
       </c>
       <c r="C16" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D16" s="3">
-        <v>235</v>
       </c>
       <c r="E16" s="3">
         <v>151</v>
@@ -769,9 +703,6 @@
       <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="3">
-        <v>183561</v>
-      </c>
       <c r="E18" s="3">
         <v>217068</v>
       </c>
@@ -783,9 +714,6 @@
       <c r="C19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="3">
-        <v>100</v>
-      </c>
       <c r="E19" s="3">
         <v>161</v>
       </c>
@@ -797,9 +725,6 @@
       <c r="C20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="3">
-        <v>194591</v>
-      </c>
       <c r="E20" s="3">
         <v>217076</v>
       </c>
@@ -811,9 +736,6 @@
       <c r="C21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="3">
-        <v>184538</v>
-      </c>
       <c r="E21" s="3">
         <v>217316</v>
       </c>
@@ -825,9 +747,6 @@
       <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="3">
-        <v>1685</v>
-      </c>
       <c r="E22" s="3">
         <v>2193</v>
       </c>
@@ -839,9 +758,6 @@
       <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="3">
-        <v>1787</v>
-      </c>
       <c r="E23" s="3">
         <v>2200</v>
       </c>
@@ -852,9 +768,6 @@
       </c>
       <c r="C24" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D24" s="3">
-        <v>245</v>
       </c>
       <c r="E24" s="3">
         <v>156</v>
@@ -876,9 +789,6 @@
       <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="3">
-        <v>4974</v>
-      </c>
       <c r="E26" s="3">
         <v>8313</v>
       </c>
@@ -890,9 +800,6 @@
       <c r="C27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="3">
-        <v>100000000</v>
-      </c>
       <c r="E27" s="3" t="s">
         <v>31</v>
       </c>
@@ -903,9 +810,6 @@
       </c>
       <c r="C28" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D28" s="3">
-        <v>501</v>
       </c>
       <c r="E28" s="3">
         <v>653</v>
@@ -927,9 +831,6 @@
       <c r="C30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="3">
-        <v>2803</v>
-      </c>
       <c r="E30" s="3">
         <v>30279</v>
       </c>
@@ -940,9 +841,6 @@
       </c>
       <c r="C31" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D31" s="3">
-        <v>329</v>
       </c>
       <c r="E31" s="3">
         <v>223</v>
@@ -964,9 +862,6 @@
       <c r="C33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="3">
-        <v>600</v>
-      </c>
       <c r="E33" s="3">
         <v>87348</v>
       </c>
@@ -977,9 +872,6 @@
       </c>
       <c r="C34" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D34" s="3">
-        <v>27</v>
       </c>
       <c r="E34" s="3">
         <v>251</v>

</xml_diff>

<commit_message>
Add results from Kansas City 2017.
</commit_message>
<xml_diff>
--- a/DemoResults.xlsx
+++ b/DemoResults.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -281,6 +281,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -316,6 +333,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -497,8 +531,8 @@
   </sheetPr>
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -540,7 +574,9 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3">
+        <v>15306</v>
+      </c>
       <c r="E3" s="3">
         <v>24421</v>
       </c>
@@ -552,7 +588,9 @@
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <v>10421</v>
+      </c>
       <c r="E4" s="3">
         <v>17668</v>
       </c>
@@ -564,7 +602,9 @@
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <v>9200</v>
+      </c>
       <c r="E5" s="3">
         <v>15058</v>
       </c>
@@ -576,7 +616,9 @@
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <v>131</v>
+      </c>
       <c r="E6" s="3">
         <v>172</v>
       </c>
@@ -597,6 +639,9 @@
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D8" s="3">
+        <v>3479</v>
+      </c>
       <c r="E8" s="3">
         <v>4098</v>
       </c>
@@ -608,6 +653,9 @@
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D9" s="3">
+        <v>3113</v>
+      </c>
       <c r="E9" s="3">
         <v>3395</v>
       </c>
@@ -619,6 +667,9 @@
       <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="D10" s="3">
+        <v>926</v>
+      </c>
       <c r="E10" s="3">
         <v>821</v>
       </c>
@@ -629,6 +680,9 @@
       </c>
       <c r="C11" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>467</v>
       </c>
       <c r="E11" s="3">
         <v>677</v>
@@ -650,6 +704,9 @@
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D13" s="3">
+        <v>3151</v>
+      </c>
       <c r="E13" s="3">
         <v>3171</v>
       </c>
@@ -661,6 +718,9 @@
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D14" s="3">
+        <v>3575</v>
+      </c>
       <c r="E14" s="3">
         <v>3188</v>
       </c>
@@ -672,6 +732,9 @@
       <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="D15" s="3">
+        <v>1416</v>
+      </c>
       <c r="E15" s="3">
         <v>1474</v>
       </c>
@@ -682,6 +745,9 @@
       </c>
       <c r="C16" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D16" s="3">
+        <v>230</v>
       </c>
       <c r="E16" s="3">
         <v>151</v>
@@ -703,6 +769,9 @@
       <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D18" s="3">
+        <v>183561</v>
+      </c>
       <c r="E18" s="3">
         <v>217068</v>
       </c>
@@ -714,6 +783,9 @@
       <c r="C19" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D19" s="3">
+        <v>116</v>
+      </c>
       <c r="E19" s="3">
         <v>161</v>
       </c>
@@ -725,6 +797,9 @@
       <c r="C20" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D20" s="3">
+        <v>194591</v>
+      </c>
       <c r="E20" s="3">
         <v>217076</v>
       </c>
@@ -736,6 +811,9 @@
       <c r="C21" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D21" s="3">
+        <v>184538</v>
+      </c>
       <c r="E21" s="3">
         <v>217316</v>
       </c>
@@ -747,6 +825,9 @@
       <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D22" s="3">
+        <v>1901</v>
+      </c>
       <c r="E22" s="3">
         <v>2193</v>
       </c>
@@ -758,6 +839,9 @@
       <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D23" s="3">
+        <v>1779</v>
+      </c>
       <c r="E23" s="3">
         <v>2200</v>
       </c>
@@ -768,6 +852,9 @@
       </c>
       <c r="C24" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="D24" s="3">
+        <v>249</v>
       </c>
       <c r="E24" s="3">
         <v>156</v>
@@ -789,6 +876,9 @@
       <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D26" s="3">
+        <v>5158</v>
+      </c>
       <c r="E26" s="3">
         <v>8313</v>
       </c>
@@ -800,6 +890,9 @@
       <c r="C27" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="D27" s="3">
+        <v>100000000</v>
+      </c>
       <c r="E27" s="3" t="s">
         <v>31</v>
       </c>
@@ -810,6 +903,9 @@
       </c>
       <c r="C28" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="D28" s="3">
+        <v>555</v>
       </c>
       <c r="E28" s="3">
         <v>653</v>
@@ -831,6 +927,9 @@
       <c r="C30" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="D30" s="3">
+        <v>2279</v>
+      </c>
       <c r="E30" s="3">
         <v>30279</v>
       </c>
@@ -841,6 +940,9 @@
       </c>
       <c r="C31" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="D31" s="3">
+        <v>565</v>
       </c>
       <c r="E31" s="3">
         <v>223</v>
@@ -862,6 +964,9 @@
       <c r="C33" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="D33" s="3">
+        <v>2739</v>
+      </c>
       <c r="E33" s="3">
         <v>87348</v>
       </c>
@@ -872,6 +977,9 @@
       </c>
       <c r="C34" s="2" t="s">
         <v>29</v>
+      </c>
+      <c r="D34" s="3">
+        <v>85</v>
       </c>
       <c r="E34" s="3">
         <v>251</v>

</xml_diff>